<commit_message>
Add ProtoBlock replacement for string block names
</commit_message>
<xml_diff>
--- a/Resources/Mappe1.xlsx
+++ b/Resources/Mappe1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yanic Gottardi\Documents\GitHub\MCUtils\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B28ACFAF-83DD-4AC2-9A91-F1788DB5A70F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C1CDAD-0721-4B6A-B4B4-07482295542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39945" yWindow="2400" windowWidth="11655" windowHeight="9150" xr2:uid="{A682593E-BD30-4FD7-8756-84A0186A1EA1}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A682593E-BD30-4FD7-8756-84A0186A1EA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="985">
   <si>
     <t>ID</t>
   </si>
@@ -2772,6 +2772,237 @@
   </si>
   <si>
     <t>bee_hive</t>
+  </si>
+  <si>
+    <t>honey_block</t>
+  </si>
+  <si>
+    <t>honeycomb_block</t>
+  </si>
+  <si>
+    <t>orange_terracotta</t>
+  </si>
+  <si>
+    <t>ancient_debris</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>basalt</t>
+  </si>
+  <si>
+    <t>netherite_block</t>
+  </si>
+  <si>
+    <t>crimson_stem</t>
+  </si>
+  <si>
+    <t>warped_stem</t>
+  </si>
+  <si>
+    <t>crimson_planks</t>
+  </si>
+  <si>
+    <t>warped_planks</t>
+  </si>
+  <si>
+    <t>crimson_sign</t>
+  </si>
+  <si>
+    <t>warped_sign</t>
+  </si>
+  <si>
+    <t>crimson_wall_sign</t>
+  </si>
+  <si>
+    <t>warped_wall_sign</t>
+  </si>
+  <si>
+    <t>crimson_slab</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>warped_slab</t>
+  </si>
+  <si>
+    <t>crimson_fence</t>
+  </si>
+  <si>
+    <t>warped_fence</t>
+  </si>
+  <si>
+    <t>crimson_fence_gate</t>
+  </si>
+  <si>
+    <t>warped_fence_gate</t>
+  </si>
+  <si>
+    <t>crimson_pressure_plate</t>
+  </si>
+  <si>
+    <t>warped_pressure_plate</t>
+  </si>
+  <si>
+    <t>crimson_button</t>
+  </si>
+  <si>
+    <t>warped_button</t>
+  </si>
+  <si>
+    <t>crimson_door</t>
+  </si>
+  <si>
+    <t>warped_door</t>
+  </si>
+  <si>
+    <t>crimson_trapdoor</t>
+  </si>
+  <si>
+    <t>warped_trapdoor</t>
+  </si>
+  <si>
+    <t>crimson_fungus</t>
+  </si>
+  <si>
+    <t>warped_mushroom</t>
+  </si>
+  <si>
+    <t>crimson_nylium</t>
+  </si>
+  <si>
+    <t>warped_nylium</t>
+  </si>
+  <si>
+    <t>crimson_roots</t>
+  </si>
+  <si>
+    <t>warped_roots</t>
+  </si>
+  <si>
+    <t>nether_sprouts</t>
+  </si>
+  <si>
+    <t>shroomlight</t>
+  </si>
+  <si>
+    <t>soul_fire</t>
+  </si>
+  <si>
+    <t>soul_lantern</t>
+  </si>
+  <si>
+    <t>soul_torch</t>
+  </si>
+  <si>
+    <t>soul_wall_torch</t>
+  </si>
+  <si>
+    <t>soul_soil</t>
+  </si>
+  <si>
+    <t>warped_wart_block</t>
+  </si>
+  <si>
+    <t>weeping_vines</t>
+  </si>
+  <si>
+    <t>crying_obsidian</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>crimson_hyphae</t>
+  </si>
+  <si>
+    <t>warped_hyphae</t>
+  </si>
+  <si>
+    <t>nether_gold_ore</t>
+  </si>
+  <si>
+    <t>twisting_vines</t>
+  </si>
+  <si>
+    <t>polished_basalt</t>
+  </si>
+  <si>
+    <t>respawn_anchor</t>
+  </si>
+  <si>
+    <t>lodestone</t>
+  </si>
+  <si>
+    <t>blackstone</t>
+  </si>
+  <si>
+    <t>blackstone_slab</t>
+  </si>
+  <si>
+    <t>blackstone_stairs</t>
+  </si>
+  <si>
+    <t>blackstone_wall</t>
+  </si>
+  <si>
+    <t>polished_blackstone_bricks</t>
+  </si>
+  <si>
+    <t>polished_blackstone</t>
+  </si>
+  <si>
+    <t>polished_blackstone_slab</t>
+  </si>
+  <si>
+    <t>polished_blackstone_wall</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>polished_blackstone_stairs</t>
+  </si>
+  <si>
+    <t>polished_blackstone_brick_slab</t>
+  </si>
+  <si>
+    <t>polished_blackstone_brick_wall</t>
+  </si>
+  <si>
+    <t>polished_blackstone_brick_stairs</t>
+  </si>
+  <si>
+    <t>polished_blackstone_button</t>
+  </si>
+  <si>
+    <t>polished_blackstone_pressure_plate</t>
+  </si>
+  <si>
+    <t>chiseled_nether_bricks</t>
+  </si>
+  <si>
+    <t>chiseled_polished_blackstone</t>
+  </si>
+  <si>
+    <t>cracked_nether_bricks</t>
+  </si>
+  <si>
+    <t>cracked_polished_blackstone_bricks</t>
+  </si>
+  <si>
+    <t>gilded_blackstone</t>
+  </si>
+  <si>
+    <t>quartz_bricks</t>
+  </si>
+  <si>
+    <t>soul_campfire</t>
+  </si>
+  <si>
+    <t>chains</t>
   </si>
 </sst>
 </file>
@@ -3134,11 +3365,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EABF65A-83D7-48CD-9DF1-1517780EE19B}">
-  <dimension ref="A1:F483"/>
+  <dimension ref="A1:F608"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D485" sqref="D485"/>
+      <pane ySplit="1" topLeftCell="A539" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F557" sqref="F557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9936,6 +10167,1123 @@
       </c>
       <c r="F483" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="E484" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="F484" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="E485" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="F485" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="E486" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F486" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="E487" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F487" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="E488" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F488" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E489" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F489" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E490" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F490" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="E491" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F491" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="E492" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F492" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E493" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F493" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E494" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F494" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A495" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E495" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F495" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A496" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E496" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F496" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A497" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E497" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F497" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A498" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E498" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F498" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A499" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E499" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F499" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A500" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E500" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F500" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A501" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A502" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F502" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="E503" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F503" s="1" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="E504" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F504" s="1" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E505" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F505" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E506" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E507" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E508" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F508" s="1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E509" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F509" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E510" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F510" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="E511" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="E512" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F512" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="E513" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F513" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="E514" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F514" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="E515" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="E517" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A518" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="E518" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F518" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A519" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F519" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E520" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F520" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="E521" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F521" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E522" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F522" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A523" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="E523" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F523" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A524" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="E524" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F524" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A525" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="E525" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A526" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="E526" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F526" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A527" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="E527" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F527" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A528" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E528" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F528" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A529" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E529" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F529" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A530" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="E530" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F530" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A531" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="E531" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A532" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="E532" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F532" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="E533" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F533" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="E534" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F534" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="E535" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F535" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E536" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F536" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A537" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="E537" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F537" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A538" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="E538" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F538" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A539" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="E539" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F539" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A540" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="E540" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F540" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A541" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E541" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F541" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A542" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="E542" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F542" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A543" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="E543" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F543" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A544" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="E544" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F544" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A545" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="E545" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F545" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A546" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="E546" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F546" s="1" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A547" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E547" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F547" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A548" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="E548" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F548" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A549" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="E549" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F549" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A550" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="E550" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F550" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A551" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="E551" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F551" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A552" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="E552" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F552" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A553" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="E553" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F553" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="E554" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F554" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="E555" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F555" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="E556" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F556" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E557" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E558" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E559" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E560" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="561" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E561" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="562" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E562" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="563" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E563" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="564" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E564" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="565" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E565" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="566" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E566" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="567" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E567" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="568" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E568" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="569" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E569" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="570" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E570" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="571" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E571" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="572" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E572" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="573" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E573" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="574" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E574" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="575" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E575" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="576" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E576" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="577" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E577" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="578" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E578" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="579" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E579" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="580" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E580" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="581" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E581" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="582" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E582" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="583" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E583" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="584" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E584" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="585" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E585" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="586" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E586" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="587" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E587" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="588" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E588" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="589" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E589" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="590" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E590" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="591" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E591" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="592" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E592" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="593" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E593" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="594" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E594" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="595" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E595" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="596" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E596" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="597" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E597" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="598" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E598" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="599" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E599" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="600" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E600" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="601" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E601" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="602" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E602" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="603" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E603" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="604" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E604" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="605" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E605" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="606" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E606" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="607" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E607" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="608" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E608" s="1" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>

</xml_diff>